<commit_message>
Adjusted Datasheet, adjusted data files derived from Datasheet
</commit_message>
<xml_diff>
--- a/data/Table_01.xlsx
+++ b/data/Table_01.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -525,7 +525,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Llano Grande</t>
+          <t>Agua Blanca PAB III</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -534,21 +534,21 @@
         </is>
       </c>
       <c r="C8">
-        <v>6.483333</v>
+        <v>5</v>
       </c>
       <c r="D8">
-        <v>-76.09999999999999</v>
+        <v>-74.09999999999999</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Velasquez &amp; Hooghiemstra ,2013</t>
+          <t>Brunschon &amp; Behling ,2009</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>El Morro</t>
+          <t>Paramo de Pena Negra 1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -557,21 +557,21 @@
         </is>
       </c>
       <c r="C9">
-        <v>6.669972</v>
+        <v>5.05</v>
       </c>
       <c r="D9">
-        <v>-75.667889</v>
+        <v>-74.05</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Velasquez Montoya ,2013</t>
+          <t>Brunschon &amp; Behling ,2009</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>El Triunfo</t>
+          <t>Agua Blanca PAB III</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -580,21 +580,21 @@
         </is>
       </c>
       <c r="C10">
-        <v>4.58545</v>
+        <v>5</v>
       </c>
       <c r="D10">
-        <v>-75.19558000000001</v>
+        <v>-74.09999999999999</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Giraldo-Giraldo et al, 2018</t>
+          <t>Niemann &amp; Behling ,2008a</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>La Laguna</t>
+          <t>Paramo de Pena Negra 1</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -603,21 +603,21 @@
         </is>
       </c>
       <c r="C11">
-        <v>4.916667</v>
+        <v>5.05</v>
       </c>
       <c r="D11">
-        <v>-74.333333</v>
+        <v>-74.05</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Villota et al., 2014</t>
+          <t>Niemann &amp; Behling ,2008a</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Paramo de Agua Blanca III</t>
+          <t>Agua Blanca PAB III</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -633,14 +633,14 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Kuhry, 1988</t>
+          <t>Rodriguez &amp; Behling ,2012</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Paramo de Laguna Verde I</t>
+          <t>Paramo de Pena Negra 1</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -649,21 +649,21 @@
         </is>
       </c>
       <c r="C13">
-        <v>5.15</v>
+        <v>5.05</v>
       </c>
       <c r="D13">
-        <v>-74</v>
+        <v>-74.05</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Kuhry, 1988</t>
+          <t>Rodriguez &amp; Behling ,2012</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Paramo de pena Negra I</t>
+          <t>Agua Blanca PAB III</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -672,21 +672,21 @@
         </is>
       </c>
       <c r="C14">
-        <v>5.05</v>
+        <v>5</v>
       </c>
       <c r="D14">
-        <v>-74.05</v>
+        <v>-74.09999999999999</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Kuhry, 1988</t>
+          <t>Rull et al ,1987</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>El Morro</t>
+          <t>Llano Grande</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -695,21 +695,21 @@
         </is>
       </c>
       <c r="C15">
-        <v>6.669972</v>
+        <v>6.483333</v>
       </c>
       <c r="D15">
-        <v>-75.667889</v>
+        <v>-76.09999999999999</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Velasquez Montoya ,2033</t>
+          <t>Velasquez &amp; Hooghiemstra ,2013</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>La Laguna</t>
+          <t>El Morro</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -718,21 +718,21 @@
         </is>
       </c>
       <c r="C16">
-        <v>4.916667</v>
+        <v>6.669972</v>
       </c>
       <c r="D16">
-        <v>-74.333333</v>
+        <v>-75.667889</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Rodriguez &amp; Behling ,2012</t>
+          <t>Velasquez Montoya ,2013</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>El Morro</t>
+          <t>El Triunfo</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -741,21 +741,21 @@
         </is>
       </c>
       <c r="C17">
-        <v>6.669972</v>
+        <v>4.58545</v>
       </c>
       <c r="D17">
-        <v>-75.667889</v>
+        <v>-75.19558000000001</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Velasquez Montoya ,2015</t>
+          <t>Giraldo-Giraldo et al, 2018</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>El Morro</t>
+          <t>El Triunfo</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -764,21 +764,21 @@
         </is>
       </c>
       <c r="C18">
-        <v>6.669972</v>
+        <v>4.58545</v>
       </c>
       <c r="D18">
-        <v>-75.667889</v>
+        <v>-75.19558000000001</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Velasquez Montoya ,2034</t>
+          <t>Giraldo-Giraldo et al, 2019</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Paramo de Laguna Verde II</t>
+          <t>Paramo de Pena Negra 1</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -787,21 +787,21 @@
         </is>
       </c>
       <c r="C19">
-        <v>5.15</v>
+        <v>5.05</v>
       </c>
       <c r="D19">
-        <v>-74</v>
+        <v>-74.05</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Brunschon &amp; Behling ,2009</t>
+          <t>Loughlin 2008</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>La Laguna</t>
+          <t>Agua Blanca PAB III</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -810,21 +810,21 @@
         </is>
       </c>
       <c r="C20">
-        <v>4.916667</v>
+        <v>5</v>
       </c>
       <c r="D20">
-        <v>-74.333333</v>
+        <v>-74.09999999999999</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Niemann &amp; Behling ,2008a</t>
+          <t>Kuhry, 1988</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>La Laguna</t>
+          <t>Paramo de Pena Negra 1</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -833,21 +833,21 @@
         </is>
       </c>
       <c r="C21">
-        <v>4.916667</v>
+        <v>5.05</v>
       </c>
       <c r="D21">
-        <v>-74.333333</v>
+        <v>-74.05</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Brunschon &amp; Behling ,2009</t>
+          <t>Kuhry, 1988</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Paramo de Laguna Verde II</t>
+          <t>Paramo de Laguna Verde I</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -863,14 +863,14 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Rodriguez &amp; Behling ,2012</t>
+          <t>Kuhry, 1988</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>El Morro</t>
+          <t>Paramo de Laguna Verde II</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -879,481 +879,484 @@
         </is>
       </c>
       <c r="C23">
-        <v>6.669972</v>
+        <v>5.15</v>
       </c>
       <c r="D23">
-        <v>-75.667889</v>
+        <v>-74</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Velasquez Montoya ,2016</t>
+          <t>Kuhry, 1988</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Paramo de Laguna Verde II</t>
+          <t>Cerro Toledo CT</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="C24">
-        <v>5.15</v>
+        <v>-4.379917</v>
       </c>
       <c r="D24">
-        <v>-74</v>
+        <v>-79.11922199999999</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Helmens et al., 1996</t>
+          <t>Brunschon &amp; Behling ,2009</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>El Morro</t>
+          <t>El Tiro</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="C25">
-        <v>6.669972</v>
+        <v>-3.840528</v>
       </c>
       <c r="D25">
-        <v>-75.667889</v>
+        <v>-79.14533299999999</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Velasquez Montoya ,2017</t>
+          <t>Brunschon &amp; Behling ,2009</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>El Morro</t>
+          <t>Lagunas Natosas Forest</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="C26">
-        <v>6.669972</v>
+        <v>-4.730417</v>
       </c>
       <c r="D26">
-        <v>-75.667889</v>
+        <v>-79.424064</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Velasquez Montoya ,2018</t>
+          <t>Brunschon &amp; Behling ,2009</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Paramo de Laguna Verde II</t>
+          <t xml:space="preserve">Huila
+</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="C27">
-        <v>5.15</v>
+        <v>-0.25405</v>
       </c>
       <c r="D27">
-        <v>-74</v>
+        <v>-78.01075</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Niemann &amp; Behling ,2008a</t>
+          <t>Brunschon &amp; Behling ,2009</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>El Morro</t>
+          <t>Cocha Caranga Laguna</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="C28">
-        <v>6.669972</v>
+        <v>-4.04375</v>
       </c>
       <c r="D28">
-        <v>-75.667889</v>
+        <v>-79.162556</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Velasquez Montoya ,2019</t>
+          <t>Niemann &amp; Behling ,2009</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>El Morro</t>
+          <t>Cocha Caranga Mire</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="C29">
-        <v>6.669972</v>
+        <v>-4.04375</v>
       </c>
       <c r="D29">
-        <v>-75.667889</v>
+        <v>-79.162556</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Velasquez Montoya ,2020</t>
+          <t>Niemann &amp; Behling ,2009</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>El Morro</t>
+          <t xml:space="preserve">Huila
+</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="C30">
-        <v>6.669972</v>
+        <v>-0.25405</v>
       </c>
       <c r="D30">
-        <v>-75.667889</v>
+        <v>-78.01075</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Velasquez Montoya ,2021</t>
+          <t>Niemann &amp; Behling ,2008a</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>El Morro</t>
+          <t>Cerro Toledo CT</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="C31">
-        <v>6.669972</v>
+        <v>-4.379917</v>
       </c>
       <c r="D31">
-        <v>-75.667889</v>
+        <v>-79.11922199999999</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Velasquez Montoya ,2022</t>
+          <t>Niemann &amp; Behling ,2008a</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>El Morro</t>
+          <t>El Tiro</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="C32">
-        <v>6.669972</v>
+        <v>-3.840528</v>
       </c>
       <c r="D32">
-        <v>-75.667889</v>
+        <v>-79.14533299999999</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Velasquez Montoya ,2023</t>
+          <t>Niemann &amp; Behling ,2008a</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>El Morro</t>
+          <t>Lagunas Natosas Forest</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="C33">
-        <v>6.669972</v>
+        <v>-4.730417</v>
       </c>
       <c r="D33">
-        <v>-75.667889</v>
+        <v>-79.424064</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Velasquez Montoya ,2014</t>
+          <t>Niemann &amp; Behling ,2008a</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>El Triunfo</t>
+          <t>G15-II</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="C34">
-        <v>4.58545</v>
+        <v>0.6</v>
       </c>
       <c r="D34">
-        <v>-75.19558000000001</v>
+        <v>-77.7</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Giraldo-Giraldo et al, 2019</t>
+          <t>Bakker et al ,2008</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>El Morro</t>
+          <t>Laguna Zurita</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="C35">
-        <v>6.669972</v>
+        <v>-3.974667</v>
       </c>
       <c r="D35">
-        <v>-75.667889</v>
+        <v>-79.117611</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Velasquez Montoya ,2024</t>
+          <t>Niemann &amp; Behling ,2010</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>El Morro</t>
+          <t>El Tiro</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="C36">
-        <v>6.669972</v>
+        <v>-3.840528</v>
       </c>
       <c r="D36">
-        <v>-75.667889</v>
+        <v>-79.14533299999999</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Velasquez Montoya ,2025</t>
+          <t>Rodriguez &amp; Behling ,2012</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>El Morro</t>
+          <t>Lagunas Natosas Forest</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="C37">
-        <v>6.669972</v>
+        <v>-4.730417</v>
       </c>
       <c r="D37">
-        <v>-75.667889</v>
+        <v>-79.424064</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Velasquez Montoya ,2026</t>
+          <t>Rodriguez &amp; Behling ,2012</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>El Morro</t>
+          <t xml:space="preserve">Huila
+</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="C38">
-        <v>6.669972</v>
+        <v>-0.25405</v>
       </c>
       <c r="D38">
-        <v>-75.667889</v>
+        <v>-78.01075</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Velasquez Montoya ,2027</t>
+          <t>Rodriguez &amp; Behling ,2012</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>El Morro</t>
+          <t>Cerro Toledo CT</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="C39">
-        <v>6.669972</v>
+        <v>-4.379917</v>
       </c>
       <c r="D39">
-        <v>-75.667889</v>
+        <v>-79.11922199999999</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Velasquez Montoya ,2028</t>
+          <t>Rodriguez &amp; Behling ,2012</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>El Morro</t>
+          <t>Pantano de Pecho</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="C40">
-        <v>6.669972</v>
+        <v>-0.333333</v>
       </c>
       <c r="D40">
-        <v>-75.667889</v>
+        <v>-79.216667</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Velasquez Montoya ,2029</t>
+          <t>Wille et al ,2002</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>El Morro</t>
+          <t>Laguna Natosa Bog</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="C41">
-        <v>6.669972</v>
+        <v>-4.732389</v>
       </c>
       <c r="D41">
-        <v>-75.667889</v>
+        <v>-79.428111</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Velasquez Montoya ,2030</t>
+          <t>Villota et al ,2012</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>El Morro</t>
+          <t>Rabadilla de Vaca</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="C42">
-        <v>6.669972</v>
+        <v>-4.255472</v>
       </c>
       <c r="D42">
-        <v>-75.667889</v>
+        <v>-79.112139</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Velasquez Montoya ,2031</t>
+          <t>Niemann et al ,2009</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>El Morro</t>
+          <t>Rabadilla de Vaca bog</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="C43">
-        <v>6.669972</v>
+        <v>-4.256583</v>
       </c>
       <c r="D43">
-        <v>-75.667889</v>
+        <v>-79.12091700000001</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Velasquez Montoya ,2032</t>
+          <t>Rodriguez &amp; Behling ,2011</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Cerro Toledo CT</t>
+          <t>Reserve Guandera-G8</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1362,21 +1365,21 @@
         </is>
       </c>
       <c r="C44">
-        <v>-4.379917</v>
+        <v>0.6</v>
       </c>
       <c r="D44">
-        <v>-79.11922199999999</v>
+        <v>-77.7</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Brunschon &amp; Behling ,2009</t>
+          <t>Moscol Olivera &amp; Hooghiemstra ,2010</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Cocha Caranga Laguna</t>
+          <t>Tres Lagunas</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1385,21 +1388,21 @@
         </is>
       </c>
       <c r="C45">
-        <v>-4.04375</v>
+        <v>-3.033333</v>
       </c>
       <c r="D45">
-        <v>-79.162556</v>
+        <v>-79.233333</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Niemann &amp; Behling ,2009</t>
+          <t>Jantz &amp; Behling ,2012</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Cocha Caranga Mire</t>
+          <t>Valle Pequeno</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1408,21 +1411,22 @@
         </is>
       </c>
       <c r="C46">
-        <v>-4.04375</v>
+        <v>-4.116083</v>
       </c>
       <c r="D46">
-        <v>-79.162556</v>
+        <v>-79.172056</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Niemann &amp; Behling ,2009</t>
+          <t>Rodriguez &amp; Behling ,2011</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>El Tiro</t>
+          <t xml:space="preserve">Huila
+</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1431,21 +1435,21 @@
         </is>
       </c>
       <c r="C47">
-        <v>-3.840528</v>
+        <v>-0.25405</v>
       </c>
       <c r="D47">
-        <v>-79.14533299999999</v>
+        <v>-78.01075</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Niemann &amp; Behling ,2008a</t>
+          <t>Rull et al ,1987</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>G15-II</t>
+          <t>ECSF Cerro de Consuelo</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1454,21 +1458,21 @@
         </is>
       </c>
       <c r="C48">
-        <v>0.6</v>
+        <v>-4.002444</v>
       </c>
       <c r="D48">
-        <v>-77.7</v>
+        <v>-79.059583</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Bakker et al ,2008</t>
+          <t>Niemann &amp; Behling ,2010</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Laguna Zurita</t>
+          <t>Laguna Daniel Alvarez</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1477,21 +1481,21 @@
         </is>
       </c>
       <c r="C49">
-        <v>-3.974667</v>
+        <v>-4.018694</v>
       </c>
       <c r="D49">
-        <v>-79.117611</v>
+        <v>-79.21169399999999</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Niemann &amp; Behling ,2010</t>
+          <t>Niemann et al ,2013</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Lagunas Natosas Forest</t>
+          <t>Reserve Guandera-G7</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1500,21 +1504,21 @@
         </is>
       </c>
       <c r="C50">
-        <v>-4.730417</v>
+        <v>0.6</v>
       </c>
       <c r="D50">
-        <v>-79.424064</v>
+        <v>-77.7</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Rodriguez &amp; Behling ,2012</t>
+          <t>Moscol Olivera &amp; Hooghiemstra ,2010</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Pantano de Pecho</t>
+          <t>El Cristal</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1523,21 +1527,21 @@
         </is>
       </c>
       <c r="C51">
-        <v>-0.333333</v>
+        <v>-3.860694</v>
       </c>
       <c r="D51">
-        <v>-79.216667</v>
+        <v>-79.061139</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Wille et al ,2002</t>
+          <t>Villota &amp; Behling ,2013</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Laguna Natosa Bog</t>
+          <t>Papallacta PA 1-08</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1546,21 +1550,21 @@
         </is>
       </c>
       <c r="C52">
-        <v>-4.732389</v>
+        <v>-0.358333</v>
       </c>
       <c r="D52">
-        <v>-79.428111</v>
+        <v>-78.193611</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Villota et al ,2012</t>
+          <t>Ledru et al ,2013</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Rabadilla de Vaca</t>
+          <t>Tres Lagunas</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1569,21 +1573,22 @@
         </is>
       </c>
       <c r="C53">
-        <v>-4.255472</v>
+        <v>-3.033333</v>
       </c>
       <c r="D53">
-        <v>-79.112139</v>
+        <v>-79.233333</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Niemann et al ,2009</t>
+          <t xml:space="preserve">Frederik et al, 2018
+</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Rabadilla de Vaca bog</t>
+          <t>Anteojos Valley</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1592,21 +1597,21 @@
         </is>
       </c>
       <c r="C54">
-        <v>-4.256583</v>
+        <v>-0.57946</v>
       </c>
       <c r="D54">
-        <v>-79.12091700000001</v>
+        <v>-78.24397</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Rodriguez &amp; Behling ,2011</t>
+          <t>Villota et al., 2014</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Reserve Guandera-G8</t>
+          <t>Cerro Toledo CT</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1615,21 +1620,21 @@
         </is>
       </c>
       <c r="C55">
-        <v>0.6</v>
+        <v>-4.379917</v>
       </c>
       <c r="D55">
-        <v>-77.7</v>
+        <v>-79.11922199999999</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Moscol Olivera &amp; Hooghiemstra ,2010</t>
+          <t>Kuhry, 1988</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Tres Lagunas</t>
+          <t>El Tiro</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1638,21 +1643,21 @@
         </is>
       </c>
       <c r="C56">
-        <v>-3.033333</v>
+        <v>-3.840528</v>
       </c>
       <c r="D56">
-        <v>-79.233333</v>
+        <v>-79.14533299999999</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Jantz &amp; Behling ,2012</t>
+          <t>Kuhry, 1988</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Valle Pequeno</t>
+          <t>Lagunas Natosas Forest</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1661,21 +1666,22 @@
         </is>
       </c>
       <c r="C57">
-        <v>-4.116083</v>
+        <v>-4.730417</v>
       </c>
       <c r="D57">
-        <v>-79.172056</v>
+        <v>-79.424064</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Rodriguez &amp; Behling ,2011</t>
+          <t>Kuhry, 1988</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>ECSF Cerro de Consuelo</t>
+          <t xml:space="preserve">Huila
+</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1684,774 +1690,129 @@
         </is>
       </c>
       <c r="C58">
-        <v>-4.002444</v>
+        <v>-0.25405</v>
       </c>
       <c r="D58">
-        <v>-79.059583</v>
+        <v>-78.01075</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Niemann &amp; Behling ,2010</t>
+          <t>Kuhry, 1988</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Laguna Daniel Alvarez</t>
+          <t>Piedras Blancas</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="C59">
-        <v>-4.018694</v>
+        <v>9.166667</v>
       </c>
       <c r="D59">
-        <v>-79.21169399999999</v>
+        <v>-70.833333</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Niemann et al ,2013</t>
+          <t>Brunschon &amp; Behling ,2009</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Reserve Guandera-G7</t>
+          <t>Piedras Blancas</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="C60">
-        <v>0.6</v>
+        <v>9.166667</v>
       </c>
       <c r="D60">
-        <v>-77.7</v>
+        <v>-70.833333</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Moscol Olivera &amp; Hooghiemstra ,2010</t>
+          <t>Niemann &amp; Behling ,2008a</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>El Cristal</t>
+          <t>Piedras Blancas</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="C61">
-        <v>-3.860694</v>
+        <v>9.166667</v>
       </c>
       <c r="D61">
-        <v>-79.061139</v>
+        <v>-70.833333</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Villota &amp; Behling ,2013</t>
+          <t>Rodriguez &amp; Behling ,2012</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Papallacta PA 1-08</t>
+          <t>Laguna Verde Alta</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="C62">
-        <v>-0.358333</v>
+        <v>8.852608</v>
       </c>
       <c r="D62">
-        <v>-78.193611</v>
+        <v>-70.87415</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Ledru et al ,2013</t>
+          <t>Rull et al ,2005c</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Tres Lagunas</t>
+          <t>Piedras Blancas</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="C63">
-        <v>-3.033333</v>
+        <v>9.166667</v>
       </c>
       <c r="D63">
-        <v>-79.233333</v>
+        <v>-70.833333</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t xml:space="preserve">Frederik et al, 2018_x000D_
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>Huila</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>Ecuador</t>
-        </is>
-      </c>
-      <c r="C64">
-        <v>-0.25405</v>
-      </c>
-      <c r="D64">
-        <v>-78.01075</v>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>Loughlin 2008</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>Cerro Toledo CT</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>Ecuador</t>
-        </is>
-      </c>
-      <c r="C65">
-        <v>-4.379917</v>
-      </c>
-      <c r="D65">
-        <v>-79.11922199999999</v>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
           <t>Kuhry, 1988</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>El Tiro</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>Ecuador</t>
-        </is>
-      </c>
-      <c r="C66">
-        <v>-3.840528</v>
-      </c>
-      <c r="D66">
-        <v>-79.14533299999999</v>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>Brunschon &amp; Behling ,2009</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>Lagunas Natosas Forest</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>Ecuador</t>
-        </is>
-      </c>
-      <c r="C67">
-        <v>-4.730417</v>
-      </c>
-      <c r="D67">
-        <v>-79.424064</v>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>Niemann &amp; Behling ,2008a</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>Cerro Toledo CT</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>Ecuador</t>
-        </is>
-      </c>
-      <c r="C68">
-        <v>-4.379917</v>
-      </c>
-      <c r="D68">
-        <v>-79.11922199999999</v>
-      </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>Villota et al., 2014</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>El Tiro</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>Ecuador</t>
-        </is>
-      </c>
-      <c r="C69">
-        <v>-3.840528</v>
-      </c>
-      <c r="D69">
-        <v>-79.14533299999999</v>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>Kuhry, 1988</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>Lagunas Natosas Forest</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>Ecuador</t>
-        </is>
-      </c>
-      <c r="C70">
-        <v>-4.730417</v>
-      </c>
-      <c r="D70">
-        <v>-79.424064</v>
-      </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>Helmens et al., 1996</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>Anteojos Valley</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>Ecuador</t>
-        </is>
-      </c>
-      <c r="C71">
-        <v>-0.57946</v>
-      </c>
-      <c r="D71">
-        <v>-78.24397</v>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>Rodriguez &amp; Behling ,2012</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>Cerro Toledo CT</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>Ecuador</t>
-        </is>
-      </c>
-      <c r="C72">
-        <v>-4.379917</v>
-      </c>
-      <c r="D72">
-        <v>-79.11922199999999</v>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>Helmens et al., 1996</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>Cerro Toledo CT</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>Ecuador</t>
-        </is>
-      </c>
-      <c r="C73">
-        <v>-4.379917</v>
-      </c>
-      <c r="D73">
-        <v>-79.11922199999999</v>
-      </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>Rodriguez &amp; Behling ,2012</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>El Tiro</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>Ecuador</t>
-        </is>
-      </c>
-      <c r="C74">
-        <v>-3.840528</v>
-      </c>
-      <c r="D74">
-        <v>-79.14533299999999</v>
-      </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>Helmens et al., 1996</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>Lagunas Natosas Forest</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>Ecuador</t>
-        </is>
-      </c>
-      <c r="C75">
-        <v>-4.730417</v>
-      </c>
-      <c r="D75">
-        <v>-79.424064</v>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>Brunschon &amp; Behling ,2009</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>Cerro Toledo CT</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>Ecuador</t>
-        </is>
-      </c>
-      <c r="C76">
-        <v>-4.379917</v>
-      </c>
-      <c r="D76">
-        <v>-79.11922199999999</v>
-      </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>Niemann &amp; Behling ,2008a</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>El Tiro</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>Ecuador</t>
-        </is>
-      </c>
-      <c r="C77">
-        <v>-3.840528</v>
-      </c>
-      <c r="D77">
-        <v>-79.14533299999999</v>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>Rodriguez &amp; Behling ,2012</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>Anteojos Valley</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>Ecuador</t>
-        </is>
-      </c>
-      <c r="C78">
-        <v>-0.57946</v>
-      </c>
-      <c r="D78">
-        <v>-78.24397</v>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>Niemann &amp; Behling ,2008a</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>El Tiro</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>Ecuador</t>
-        </is>
-      </c>
-      <c r="C79">
-        <v>-3.840528</v>
-      </c>
-      <c r="D79">
-        <v>-79.14533299999999</v>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>Villota et al., 2014</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>Lagunas Natosas Forest</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>Ecuador</t>
-        </is>
-      </c>
-      <c r="C80">
-        <v>-4.730417</v>
-      </c>
-      <c r="D80">
-        <v>-79.424064</v>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>Kuhry, 1988</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>Anteojos Valley</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>Ecuador</t>
-        </is>
-      </c>
-      <c r="C81">
-        <v>-0.57946</v>
-      </c>
-      <c r="D81">
-        <v>-78.24397</v>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>Helmens et al., 1996</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>Lagunas Natosas Forest</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>Ecuador</t>
-        </is>
-      </c>
-      <c r="C82">
-        <v>-4.730417</v>
-      </c>
-      <c r="D82">
-        <v>-79.424064</v>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>Villota et al., 2014</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>Anteojos Valley</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>Ecuador</t>
-        </is>
-      </c>
-      <c r="C83">
-        <v>-0.57946</v>
-      </c>
-      <c r="D83">
-        <v>-78.24397</v>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>Kuhry, 1988</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>Laguna Verde Alta</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>Venezuela</t>
-        </is>
-      </c>
-      <c r="C84">
-        <v>8.852608</v>
-      </c>
-      <c r="D84">
-        <v>-70.87415</v>
-      </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>Rull et al ,2005c</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>Piedras Blancas</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>Venezuela</t>
-        </is>
-      </c>
-      <c r="C85">
-        <v>9.166667</v>
-      </c>
-      <c r="D85">
-        <v>-70.833333</v>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>Rull et al ,1987</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>Piedras Blancas</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>Venezuela</t>
-        </is>
-      </c>
-      <c r="C86">
-        <v>9.166667</v>
-      </c>
-      <c r="D86">
-        <v>-70.833333</v>
-      </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>Helmens et al., 1996</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>Piedras Blancas</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>Venezuela</t>
-        </is>
-      </c>
-      <c r="C87">
-        <v>9.166667</v>
-      </c>
-      <c r="D87">
-        <v>-70.833333</v>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>Brunschon &amp; Behling ,2009</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>Piedras Blancas</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>Venezuela</t>
-        </is>
-      </c>
-      <c r="C88">
-        <v>9.166667</v>
-      </c>
-      <c r="D88">
-        <v>-70.833333</v>
-      </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>Niemann &amp; Behling ,2008a</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>Piedras Blancas</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>Venezuela</t>
-        </is>
-      </c>
-      <c r="C89">
-        <v>9.166667</v>
-      </c>
-      <c r="D89">
-        <v>-70.833333</v>
-      </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>Rodriguez &amp; Behling ,2012</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>Piedras Blancas</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>Venezuela</t>
-        </is>
-      </c>
-      <c r="C90">
-        <v>9.166667</v>
-      </c>
-      <c r="D90">
-        <v>-70.833333</v>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>Kuhry, 1988</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>Piedras Blancas</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>Venezuela</t>
-        </is>
-      </c>
-      <c r="C91">
-        <v>9.166667</v>
-      </c>
-      <c r="D91">
-        <v>-70.833333</v>
-      </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>Villota et al., 2014</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
figures and df adjustments
</commit_message>
<xml_diff>
--- a/data/Table_01.xlsx
+++ b/data/Table_01.xlsx
@@ -525,7 +525,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Llano Grande</t>
+          <t>Rio Timbio</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -534,21 +534,21 @@
         </is>
       </c>
       <c r="C8">
-        <v>6.483333</v>
+        <v>2.4</v>
       </c>
       <c r="D8">
-        <v>-76.09999999999999</v>
+        <v>-76.59999999999999</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Velasquez &amp; Hooghiemstra ,2013</t>
+          <t>Wille et al ,2000</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>El Morro</t>
+          <t>Llano Grande</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -557,21 +557,21 @@
         </is>
       </c>
       <c r="C9">
-        <v>6.669972</v>
+        <v>6.483333</v>
       </c>
       <c r="D9">
-        <v>-75.667889</v>
+        <v>-76.09999999999999</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Velasquez Montoya ,2013</t>
+          <t>Velasquez &amp; Hooghiemstra ,2013</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>El Triunfo</t>
+          <t>El Morro</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -580,14 +580,14 @@
         </is>
       </c>
       <c r="C10">
-        <v>4.58545</v>
+        <v>6.669972</v>
       </c>
       <c r="D10">
-        <v>-75.19558000000001</v>
+        <v>-75.667889</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Giraldo-Giraldo et al, 2018</t>
+          <t>Velasquez Montoya ,2013</t>
         </is>
       </c>
     </row>
@@ -610,7 +610,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Giraldo-Giraldo et al, 2019</t>
+          <t>Giraldo-Giraldo et al, 2018</t>
         </is>
       </c>
     </row>
@@ -629,7 +629,7 @@
         <v>5</v>
       </c>
       <c r="D12">
-        <v>-74.09999999999999</v>
+        <v>-74.166667</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -649,7 +649,7 @@
         </is>
       </c>
       <c r="C13">
-        <v>5.15</v>
+        <v>5.25</v>
       </c>
       <c r="D13">
         <v>-74</v>
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="C14">
-        <v>5.15</v>
+        <v>5.25</v>
       </c>
       <c r="D14">
         <v>-74</v>
@@ -695,10 +695,10 @@
         </is>
       </c>
       <c r="C15">
-        <v>5.05</v>
+        <v>5.083333</v>
       </c>
       <c r="D15">
-        <v>-74.05</v>
+        <v>-74.083333</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -1146,7 +1146,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Tres Lagunas</t>
+          <t>Tres Lagunas (2)</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1155,14 +1155,14 @@
         </is>
       </c>
       <c r="C35">
-        <v>-3.033333</v>
+        <v>-3.05145</v>
       </c>
       <c r="D35">
-        <v>-79.233333</v>
+        <v>-79.24822</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Frederik et al, 2018
+          <t xml:space="preserve">Frederik et al, 2018_x000D__x000D_
 </t>
         </is>
       </c>
@@ -1193,7 +1193,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Huila
+          <t xml:space="preserve">Huila_x000D__x000D_
 </t>
         </is>
       </c>
@@ -1203,7 +1203,7 @@
         </is>
       </c>
       <c r="C37">
-        <v>-0.25405</v>
+        <v>0.25405</v>
       </c>
       <c r="D37">
         <v>-78.01075</v>

</xml_diff>